<commit_message>
lnCS6 to log CS6 update
</commit_message>
<xml_diff>
--- a/docs/Examples/Mantle_Melting_Lee_Wieser/Thermocalc_Melting_Path.xlsx
+++ b/docs/Examples/Mantle_Melting_Lee_Wieser/Thermocalc_Melting_Path.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\PySulfSat\PySulfSat_Structure\docs\Examples\Mantle_Melting_Lee_Wieser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DB2185-313F-4516-AAF3-4209FAD2FE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59630AC3-FBF5-4B5C-9C3A-6D01E0EE9AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{2CBD97AA-CD08-4B34-8E28-2055BA147178}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="38">
   <si>
     <t>depletion</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>FeOt</t>
+  </si>
+  <si>
+    <t>FeO</t>
   </si>
 </sst>
 </file>
@@ -544,7 +547,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -552,15 +555,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5A7A78-E4F0-4BB9-BF83-AD259FE01203}">
-  <dimension ref="A1:AH52"/>
+  <dimension ref="A1:AI52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:34" ht="48.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="48.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +610,7 @@
         <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q1" t="s">
         <v>15</v>
@@ -616,55 +619,58 @@
         <v>16</v>
       </c>
       <c r="S1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>5</v>
       </c>
@@ -714,22 +720,23 @@
         <v>0.54</v>
       </c>
       <c r="S2" s="7">
+        <f>P2+R2*0.8998</f>
+        <v>9.8858920000000001</v>
+      </c>
+      <c r="T2" s="7">
         <v>0.08</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="U2" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="U2" s="7">
-        <v>0</v>
       </c>
       <c r="V2" s="7">
         <v>0</v>
       </c>
       <c r="W2" s="7">
+        <v>0</v>
+      </c>
+      <c r="X2" s="7">
         <v>1094.51296614648</v>
-      </c>
-      <c r="X2" s="7">
-        <v>0</v>
       </c>
       <c r="Y2" s="7">
         <v>0</v>
@@ -738,31 +745,34 @@
         <v>0</v>
       </c>
       <c r="AA2" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="7">
         <v>1094.51296614648</v>
-      </c>
-      <c r="AB2" s="7">
-        <v>0</v>
       </c>
       <c r="AC2" s="7">
         <v>0</v>
       </c>
       <c r="AD2" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="7">
         <v>1094.51296614648</v>
-      </c>
-      <c r="AE2" s="7">
-        <v>0</v>
       </c>
       <c r="AF2" s="7">
         <v>0</v>
       </c>
       <c r="AG2" s="7">
-        <v>1094.51296614648</v>
+        <v>0</v>
       </c>
       <c r="AH2" s="7">
         <v>1094.51296614648</v>
       </c>
+      <c r="AI2" s="7">
+        <v>1094.51296614648</v>
+      </c>
     </row>
-    <row r="3" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>5</v>
       </c>
@@ -812,55 +822,59 @@
         <v>0.52</v>
       </c>
       <c r="S3" s="7">
+        <f t="shared" ref="S3:S52" si="0">P3+R3*0.8998</f>
+        <v>9.8778959999999998</v>
+      </c>
+      <c r="T3" s="7">
         <v>0.08</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="U3" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="U3" s="7">
-        <v>61.084161231220101</v>
       </c>
       <c r="V3" s="7">
         <v>61.084161231220101</v>
       </c>
       <c r="W3" s="7">
+        <v>61.084161231220101</v>
+      </c>
+      <c r="X3" s="7">
         <v>1094.51296614648</v>
       </c>
-      <c r="X3" s="7">
+      <c r="Y3" s="7">
         <v>3.8436695193545498</v>
-      </c>
-      <c r="Y3" s="7">
-        <v>69.809653095182696</v>
       </c>
       <c r="Z3" s="7">
         <v>69.809653095182696</v>
       </c>
       <c r="AA3" s="7">
+        <v>69.809653095182696</v>
+      </c>
+      <c r="AB3" s="7">
         <v>1094.51296614648</v>
-      </c>
-      <c r="AB3" s="7">
-        <v>81.443324604966804</v>
       </c>
       <c r="AC3" s="7">
         <v>81.443324604966804</v>
       </c>
       <c r="AD3" s="7">
+        <v>81.443324604966804</v>
+      </c>
+      <c r="AE3" s="7">
         <v>1094.51296614648</v>
-      </c>
-      <c r="AE3" s="7">
-        <v>97.729854875677404</v>
       </c>
       <c r="AF3" s="7">
         <v>97.729854875677404</v>
       </c>
       <c r="AG3" s="7">
-        <v>1094.51296614648</v>
+        <v>97.729854875677404</v>
       </c>
       <c r="AH3" s="7">
         <v>1094.51296614648</v>
       </c>
+      <c r="AI3" s="7">
+        <v>1094.51296614648</v>
+      </c>
     </row>
-    <row r="4" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>5</v>
       </c>
@@ -910,55 +924,59 @@
         <v>0.51</v>
       </c>
       <c r="S4" s="7">
+        <f t="shared" si="0"/>
+        <v>9.8788979999999995</v>
+      </c>
+      <c r="T4" s="7">
         <v>0.08</v>
       </c>
-      <c r="T4" s="7" t="s">
+      <c r="U4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U4" s="7">
+      <c r="V4" s="7">
         <v>61.702913265508002</v>
       </c>
-      <c r="V4" s="7">
+      <c r="W4" s="7">
         <v>61.393537248364098</v>
       </c>
-      <c r="W4" s="7">
+      <c r="X4" s="7">
         <v>1165.71349836021</v>
       </c>
-      <c r="X4" s="7">
+      <c r="Y4" s="7">
         <v>3.7396211406458999</v>
       </c>
-      <c r="Y4" s="7">
+      <c r="Z4" s="7">
         <v>70.607880552832398</v>
       </c>
-      <c r="Z4" s="7">
+      <c r="AA4" s="7">
         <v>70.208766824007498</v>
       </c>
-      <c r="AA4" s="7">
+      <c r="AB4" s="7">
         <v>1165.71349836021</v>
       </c>
-      <c r="AB4" s="7">
+      <c r="AC4" s="7">
         <v>82.5178351662083</v>
       </c>
-      <c r="AC4" s="7">
+      <c r="AD4" s="7">
         <v>81.980579885587602</v>
       </c>
-      <c r="AD4" s="7">
+      <c r="AE4" s="7">
         <v>1165.71349836021</v>
       </c>
-      <c r="AE4" s="7">
+      <c r="AF4" s="7">
         <v>99.263589720939606</v>
       </c>
-      <c r="AF4" s="7">
+      <c r="AG4" s="7">
         <v>98.496722298308498</v>
       </c>
-      <c r="AG4" s="7">
+      <c r="AH4" s="7">
         <v>1165.71349836021</v>
       </c>
-      <c r="AH4" s="7">
+      <c r="AI4" s="7">
         <v>1236.91403057394</v>
       </c>
     </row>
-    <row r="5" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>5</v>
       </c>
@@ -1008,55 +1026,59 @@
         <v>0.5</v>
       </c>
       <c r="S5" s="7">
+        <f t="shared" si="0"/>
+        <v>9.8798999999999992</v>
+      </c>
+      <c r="T5" s="7">
         <v>0.09</v>
       </c>
-      <c r="T5" s="7" t="s">
+      <c r="U5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U5" s="7">
+      <c r="V5" s="7">
         <v>62.378411953054602</v>
       </c>
-      <c r="V5" s="7">
+      <c r="W5" s="7">
         <v>61.721828816594197</v>
       </c>
-      <c r="W5" s="7">
+      <c r="X5" s="7">
         <v>1196.2537028468</v>
       </c>
-      <c r="X5" s="7">
+      <c r="Y5" s="7">
         <v>3.6386953285008601</v>
       </c>
-      <c r="Y5" s="7">
+      <c r="Z5" s="7">
         <v>71.485601724944999</v>
       </c>
-      <c r="Z5" s="7">
+      <c r="AA5" s="7">
         <v>70.634378457653398</v>
       </c>
-      <c r="AA5" s="7">
+      <c r="AB5" s="7">
         <v>1196.2537028468</v>
       </c>
-      <c r="AB5" s="7">
+      <c r="AC5" s="7">
         <v>83.710620894485103</v>
       </c>
-      <c r="AC5" s="7">
+      <c r="AD5" s="7">
         <v>82.557260221886807</v>
       </c>
-      <c r="AD5" s="7">
+      <c r="AE5" s="7">
         <v>1196.2537028468</v>
       </c>
-      <c r="AE5" s="7">
+      <c r="AF5" s="7">
         <v>100.98888201779501</v>
       </c>
-      <c r="AF5" s="7">
+      <c r="AG5" s="7">
         <v>99.327442204803901</v>
       </c>
-      <c r="AG5" s="7">
+      <c r="AH5" s="7">
         <v>1196.2537028468</v>
       </c>
-      <c r="AH5" s="7">
+      <c r="AI5" s="7">
         <v>1257.3341118199601</v>
       </c>
     </row>
-    <row r="6" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1106,55 +1128,59 @@
         <v>0.49</v>
       </c>
       <c r="S6" s="7">
+        <f t="shared" si="0"/>
+        <v>9.880901999999999</v>
+      </c>
+      <c r="T6" s="7">
         <v>0.09</v>
       </c>
-      <c r="T6" s="7" t="s">
+      <c r="U6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U6" s="7">
+      <c r="V6" s="7">
         <v>63.096101847228198</v>
       </c>
-      <c r="V6" s="7">
+      <c r="W6" s="7">
         <v>62.065397074252701</v>
       </c>
-      <c r="W6" s="7">
+      <c r="X6" s="7">
         <v>1213.7274306386701</v>
       </c>
-      <c r="X6" s="7">
+      <c r="Y6" s="7">
         <v>3.5408084427436202</v>
       </c>
-      <c r="Y6" s="7">
+      <c r="Z6" s="7">
         <v>72.424975288423397</v>
       </c>
-      <c r="Z6" s="7">
+      <c r="AA6" s="7">
         <v>71.082027665345905</v>
       </c>
-      <c r="AA6" s="7">
+      <c r="AB6" s="7">
         <v>1213.7274306386701</v>
       </c>
-      <c r="AB6" s="7">
+      <c r="AC6" s="7">
         <v>84.999914388205099</v>
       </c>
-      <c r="AC6" s="7">
+      <c r="AD6" s="7">
         <v>83.167923763466305</v>
       </c>
-      <c r="AD6" s="7">
+      <c r="AE6" s="7">
         <v>1213.7274306386701</v>
       </c>
-      <c r="AE6" s="7">
+      <c r="AF6" s="7">
         <v>102.880675903331</v>
       </c>
-      <c r="AF6" s="7">
+      <c r="AG6" s="7">
         <v>100.215750629436</v>
       </c>
-      <c r="AG6" s="7">
+      <c r="AH6" s="7">
         <v>1213.7274306386701</v>
       </c>
-      <c r="AH6" s="7">
+      <c r="AI6" s="7">
         <v>1266.1486140142799</v>
       </c>
     </row>
-    <row r="7" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -1204,55 +1230,59 @@
         <v>0.48</v>
       </c>
       <c r="S7" s="7">
+        <f t="shared" si="0"/>
+        <v>9.8719039999999989</v>
+      </c>
+      <c r="T7" s="7">
         <v>0.09</v>
       </c>
-      <c r="T7" s="7" t="s">
+      <c r="U7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U7" s="7">
+      <c r="V7" s="7">
         <v>63.672553497939603</v>
       </c>
-      <c r="V7" s="7">
+      <c r="W7" s="7">
         <v>62.386828358990101</v>
       </c>
-      <c r="W7" s="7">
+      <c r="X7" s="7">
         <v>1225.17673740706</v>
       </c>
-      <c r="X7" s="7">
+      <c r="Y7" s="7">
         <v>3.4458785982708999</v>
       </c>
-      <c r="Y7" s="7">
+      <c r="Z7" s="7">
         <v>73.221707134174395</v>
       </c>
-      <c r="Z7" s="7">
+      <c r="AA7" s="7">
         <v>71.509963559111597</v>
       </c>
-      <c r="AA7" s="7">
+      <c r="AB7" s="7">
         <v>1225.17673740706</v>
       </c>
-      <c r="AB7" s="7">
+      <c r="AC7" s="7">
         <v>86.157364208143605</v>
       </c>
-      <c r="AC7" s="7">
+      <c r="AD7" s="7">
         <v>83.765811852401797</v>
       </c>
-      <c r="AD7" s="7">
+      <c r="AE7" s="7">
         <v>1225.17673740706</v>
       </c>
-      <c r="AE7" s="7">
+      <c r="AF7" s="7">
         <v>104.686645384028</v>
       </c>
-      <c r="AF7" s="7">
+      <c r="AG7" s="7">
         <v>101.10992958035401</v>
       </c>
-      <c r="AG7" s="7">
+      <c r="AH7" s="7">
         <v>1225.17673740706</v>
       </c>
-      <c r="AH7" s="7">
+      <c r="AI7" s="7">
         <v>1270.97396448064</v>
       </c>
     </row>
-    <row r="8" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1302,55 +1332,59 @@
         <v>0.47</v>
       </c>
       <c r="S8" s="7">
+        <f t="shared" si="0"/>
+        <v>9.8629059999999988</v>
+      </c>
+      <c r="T8" s="7">
         <v>0.1</v>
       </c>
-      <c r="T8" s="7" t="s">
+      <c r="U8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U8" s="7">
+      <c r="V8" s="7">
         <v>64.415960691095506</v>
       </c>
-      <c r="V8" s="7">
+      <c r="W8" s="7">
         <v>62.725017081007699</v>
       </c>
-      <c r="W8" s="7">
+      <c r="X8" s="7">
         <v>1234.7054019704401</v>
       </c>
-      <c r="X8" s="7">
+      <c r="Y8" s="7">
         <v>3.3538256408373899</v>
       </c>
-      <c r="Y8" s="7">
+      <c r="Z8" s="7">
         <v>74.226666532211397</v>
       </c>
-      <c r="Z8" s="7">
+      <c r="AA8" s="7">
         <v>71.962747387961599</v>
       </c>
-      <c r="AA8" s="7">
+      <c r="AB8" s="7">
         <v>1234.7054019704401</v>
       </c>
-      <c r="AB8" s="7">
+      <c r="AC8" s="7">
         <v>87.591620830846495</v>
       </c>
-      <c r="AC8" s="7">
+      <c r="AD8" s="7">
         <v>84.403446682142601</v>
       </c>
-      <c r="AD8" s="7">
+      <c r="AE8" s="7">
         <v>1234.7054019704401</v>
       </c>
-      <c r="AE8" s="7">
+      <c r="AF8" s="7">
         <v>106.900744507539</v>
       </c>
-      <c r="AF8" s="7">
+      <c r="AG8" s="7">
         <v>102.075065401552</v>
       </c>
-      <c r="AG8" s="7">
+      <c r="AH8" s="7">
         <v>1234.7054019704401</v>
       </c>
-      <c r="AH8" s="7">
+      <c r="AI8" s="7">
         <v>1282.3487247873099</v>
       </c>
     </row>
-    <row r="9" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>5</v>
       </c>
@@ -1400,55 +1434,59 @@
         <v>0.46</v>
       </c>
       <c r="S9" s="7">
+        <f t="shared" si="0"/>
+        <v>9.8539079999999988</v>
+      </c>
+      <c r="T9" s="7">
         <v>0.1</v>
       </c>
-      <c r="T9" s="7" t="s">
+      <c r="U9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U9" s="7">
+      <c r="V9" s="7">
         <v>65.208804326229199</v>
       </c>
-      <c r="V9" s="7">
+      <c r="W9" s="7">
         <v>63.079843830324997</v>
       </c>
-      <c r="W9" s="7">
+      <c r="X9" s="7">
         <v>1242.1994047542701</v>
       </c>
-      <c r="X9" s="7">
+      <c r="Y9" s="7">
         <v>3.2645711229800201</v>
       </c>
-      <c r="Y9" s="7">
+      <c r="Z9" s="7">
         <v>75.308481990685607</v>
       </c>
-      <c r="Z9" s="7">
+      <c r="AA9" s="7">
         <v>72.440709474065002</v>
       </c>
-      <c r="AA9" s="7">
+      <c r="AB9" s="7">
         <v>1242.1994047542701</v>
       </c>
-      <c r="AB9" s="7">
+      <c r="AC9" s="7">
         <v>89.156333192267098</v>
       </c>
-      <c r="AC9" s="7">
+      <c r="AD9" s="7">
         <v>85.082430469303205</v>
       </c>
-      <c r="AD9" s="7">
+      <c r="AE9" s="7">
         <v>1242.1994047542701</v>
       </c>
-      <c r="AE9" s="7">
+      <c r="AF9" s="7">
         <v>109.366981323689</v>
       </c>
-      <c r="AF9" s="7">
+      <c r="AG9" s="7">
         <v>103.116767676143</v>
       </c>
-      <c r="AG9" s="7">
+      <c r="AH9" s="7">
         <v>1242.1994047542701</v>
       </c>
-      <c r="AH9" s="7">
+      <c r="AI9" s="7">
         <v>1287.16342145727</v>
       </c>
     </row>
-    <row r="10" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>5</v>
       </c>
@@ -1498,55 +1536,59 @@
         <v>0.45</v>
       </c>
       <c r="S10" s="7">
+        <f t="shared" si="0"/>
+        <v>9.8449099999999987</v>
+      </c>
+      <c r="T10" s="7">
         <v>0.11</v>
       </c>
-      <c r="T10" s="7" t="s">
+      <c r="U10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U10" s="7">
+      <c r="V10" s="7">
         <v>66.071951104195705</v>
       </c>
-      <c r="V10" s="7">
+      <c r="W10" s="7">
         <v>63.4538572395589</v>
       </c>
-      <c r="W10" s="7">
+      <c r="X10" s="7">
         <v>1249.3309349343499</v>
       </c>
-      <c r="X10" s="7">
+      <c r="Y10" s="7">
         <v>3.1780382800814202</v>
       </c>
-      <c r="Y10" s="7">
+      <c r="Z10" s="7">
         <v>76.498405259877899</v>
       </c>
-      <c r="Z10" s="7">
+      <c r="AA10" s="7">
         <v>72.947921447291606</v>
       </c>
-      <c r="AA10" s="7">
+      <c r="AB10" s="7">
         <v>1249.3309349343499</v>
       </c>
-      <c r="AB10" s="7">
+      <c r="AC10" s="7">
         <v>90.903493497298498</v>
       </c>
-      <c r="AC10" s="7">
+      <c r="AD10" s="7">
         <v>85.810063347802597</v>
       </c>
-      <c r="AD10" s="7">
+      <c r="AE10" s="7">
         <v>1249.3309349343499</v>
       </c>
-      <c r="AE10" s="7">
+      <c r="AF10" s="7">
         <v>112.187896063655</v>
       </c>
-      <c r="AF10" s="7">
+      <c r="AG10" s="7">
         <v>104.250658724582</v>
       </c>
-      <c r="AG10" s="7">
+      <c r="AH10" s="7">
         <v>1249.3309349343499</v>
       </c>
-      <c r="AH10" s="7">
+      <c r="AI10" s="7">
         <v>1299.2516461948901</v>
       </c>
     </row>
-    <row r="11" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>5</v>
       </c>
@@ -1596,55 +1638,59 @@
         <v>0.44</v>
       </c>
       <c r="S11" s="7">
+        <f t="shared" si="0"/>
+        <v>9.8359120000000004</v>
+      </c>
+      <c r="T11" s="7">
         <v>0.11</v>
       </c>
-      <c r="T11" s="7" t="s">
+      <c r="U11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U11" s="7">
+      <c r="V11" s="7">
         <v>67.003527349383802</v>
       </c>
-      <c r="V11" s="7">
+      <c r="W11" s="7">
         <v>63.848265029539398</v>
       </c>
-      <c r="W11" s="7">
+      <c r="X11" s="7">
         <v>1255.7168682998099</v>
       </c>
-      <c r="X11" s="7">
+      <c r="Y11" s="7">
         <v>3.0941520065730801</v>
       </c>
-      <c r="Y11" s="7">
+      <c r="Z11" s="7">
         <v>77.797442266950398</v>
       </c>
-      <c r="Z11" s="7">
+      <c r="AA11" s="7">
         <v>73.486757093920403</v>
       </c>
-      <c r="AA11" s="7">
+      <c r="AB11" s="7">
         <v>1255.7168682998099</v>
       </c>
-      <c r="AB11" s="7">
+      <c r="AC11" s="7">
         <v>92.843711736931098</v>
       </c>
-      <c r="AC11" s="7">
+      <c r="AD11" s="7">
         <v>86.5915798354836</v>
       </c>
-      <c r="AD11" s="7">
+      <c r="AE11" s="7">
         <v>1255.7168682998099</v>
       </c>
-      <c r="AE11" s="7">
+      <c r="AF11" s="7">
         <v>115.41021846097701</v>
       </c>
-      <c r="AF11" s="7">
+      <c r="AG11" s="7">
         <v>105.490609806403</v>
       </c>
-      <c r="AG11" s="7">
+      <c r="AH11" s="7">
         <v>1255.7168682998099</v>
       </c>
-      <c r="AH11" s="7">
+      <c r="AI11" s="7">
         <v>1306.8043352234899</v>
       </c>
     </row>
-    <row r="12" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>5</v>
       </c>
@@ -1694,55 +1740,59 @@
         <v>0.43</v>
       </c>
       <c r="S12" s="7">
+        <f t="shared" si="0"/>
+        <v>9.8269140000000004</v>
+      </c>
+      <c r="T12" s="7">
         <v>0.12</v>
       </c>
-      <c r="T12" s="7" t="s">
+      <c r="U12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U12" s="7">
+      <c r="V12" s="7">
         <v>68.026761037684295</v>
       </c>
-      <c r="V12" s="7">
+      <c r="W12" s="7">
         <v>64.266114630353897</v>
       </c>
-      <c r="W12" s="7">
+      <c r="X12" s="7">
         <v>1262.19618402587</v>
       </c>
-      <c r="X12" s="7">
+      <c r="Y12" s="7">
         <v>3.0128388322786099</v>
       </c>
-      <c r="Y12" s="7">
+      <c r="Z12" s="7">
         <v>79.242679535329401</v>
       </c>
-      <c r="Z12" s="7">
+      <c r="AA12" s="7">
         <v>74.062349338061296</v>
       </c>
-      <c r="AA12" s="7">
+      <c r="AB12" s="7">
         <v>1262.19618402587</v>
       </c>
-      <c r="AB12" s="7">
+      <c r="AC12" s="7">
         <v>95.044931225505096</v>
       </c>
-      <c r="AC12" s="7">
+      <c r="AD12" s="7">
         <v>87.436914974485703</v>
       </c>
-      <c r="AD12" s="7">
+      <c r="AE12" s="7">
         <v>1262.19618402587</v>
       </c>
-      <c r="AE12" s="7">
+      <c r="AF12" s="7">
         <v>119.190888487808</v>
       </c>
-      <c r="AF12" s="7">
+      <c r="AG12" s="7">
         <v>106.86063767454399</v>
       </c>
-      <c r="AG12" s="7">
+      <c r="AH12" s="7">
         <v>1262.19618402587</v>
       </c>
-      <c r="AH12" s="7">
+      <c r="AI12" s="7">
         <v>1320.51002556043</v>
       </c>
     </row>
-    <row r="13" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>5</v>
       </c>
@@ -1792,55 +1842,59 @@
         <v>0.42</v>
       </c>
       <c r="S13" s="7">
+        <f t="shared" si="0"/>
+        <v>9.8079160000000005</v>
+      </c>
+      <c r="T13" s="7">
         <v>0.12</v>
       </c>
-      <c r="T13" s="7" t="s">
+      <c r="U13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U13" s="7">
+      <c r="V13" s="7">
         <v>68.699961032042395</v>
       </c>
-      <c r="V13" s="7">
+      <c r="W13" s="7">
         <v>64.669191575962003</v>
       </c>
-      <c r="W13" s="7">
+      <c r="X13" s="7">
         <v>1267.3551269607201</v>
       </c>
-      <c r="X13" s="7">
+      <c r="Y13" s="7">
         <v>2.9340268988974598</v>
       </c>
-      <c r="Y13" s="7">
+      <c r="Z13" s="7">
         <v>80.340599243937007</v>
       </c>
-      <c r="Z13" s="7">
+      <c r="AA13" s="7">
         <v>74.633099329504503</v>
       </c>
-      <c r="AA13" s="7">
+      <c r="AB13" s="7">
         <v>1267.3551269607201</v>
       </c>
-      <c r="AB13" s="7">
+      <c r="AC13" s="7">
         <v>96.963367057462307</v>
       </c>
-      <c r="AC13" s="7">
+      <c r="AD13" s="7">
         <v>88.302956072938102</v>
       </c>
-      <c r="AD13" s="7">
+      <c r="AE13" s="7">
         <v>1267.3551269607201</v>
       </c>
-      <c r="AE13" s="7">
+      <c r="AF13" s="7">
         <v>122.99574049146599</v>
       </c>
-      <c r="AF13" s="7">
+      <c r="AG13" s="7">
         <v>108.327465203355</v>
       </c>
-      <c r="AG13" s="7">
+      <c r="AH13" s="7">
         <v>1267.3551269607201</v>
       </c>
-      <c r="AH13" s="7">
+      <c r="AI13" s="7">
         <v>1318.9445563092199</v>
       </c>
     </row>
-    <row r="14" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>5</v>
       </c>
@@ -1890,55 +1944,59 @@
         <v>0.42</v>
       </c>
       <c r="S14" s="7">
+        <f t="shared" si="0"/>
+        <v>9.8079160000000005</v>
+      </c>
+      <c r="T14" s="7">
         <v>0.13</v>
       </c>
-      <c r="T14" s="7" t="s">
+      <c r="U14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U14" s="7">
+      <c r="V14" s="7">
         <v>70.365195287959395</v>
       </c>
-      <c r="V14" s="7">
+      <c r="W14" s="7">
         <v>65.143858551961699</v>
       </c>
-      <c r="W14" s="7">
+      <c r="X14" s="7">
         <v>1274.92228691471</v>
       </c>
-      <c r="X14" s="7">
+      <c r="Y14" s="7">
         <v>2.8576459366295799</v>
       </c>
-      <c r="Y14" s="7">
+      <c r="Z14" s="7">
         <v>82.634995082015195</v>
       </c>
-      <c r="Z14" s="7">
+      <c r="AA14" s="7">
         <v>75.299923975547102</v>
       </c>
-      <c r="AA14" s="7">
+      <c r="AB14" s="7">
         <v>1274.92228691471</v>
       </c>
-      <c r="AB14" s="7">
+      <c r="AC14" s="7">
         <v>100.42441187669399</v>
       </c>
-      <c r="AC14" s="7">
+      <c r="AD14" s="7">
         <v>89.313077389917794</v>
       </c>
-      <c r="AD14" s="7">
+      <c r="AE14" s="7">
         <v>1274.92228691471</v>
       </c>
-      <c r="AE14" s="7">
+      <c r="AF14" s="7">
         <v>129.11309305806901</v>
       </c>
-      <c r="AF14" s="7">
+      <c r="AG14" s="7">
         <v>110.059600857915</v>
       </c>
-      <c r="AG14" s="7">
+      <c r="AH14" s="7">
         <v>1274.92228691471</v>
       </c>
-      <c r="AH14" s="7">
+      <c r="AI14" s="7">
         <v>1358.1610464086</v>
       </c>
     </row>
-    <row r="15" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
         <v>5</v>
       </c>
@@ -1988,55 +2046,59 @@
         <v>0.41</v>
       </c>
       <c r="S15" s="7">
+        <f t="shared" si="0"/>
+        <v>9.7889180000000007</v>
+      </c>
+      <c r="T15" s="7">
         <v>0.14000000000000001</v>
       </c>
-      <c r="T15" s="7" t="s">
+      <c r="U15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U15" s="7">
+      <c r="V15" s="7">
         <v>71.201091332232295</v>
       </c>
-      <c r="V15" s="7">
+      <c r="W15" s="7">
         <v>65.609799535059494</v>
       </c>
-      <c r="W15" s="7">
+      <c r="X15" s="7">
         <v>1280.3042623915701</v>
       </c>
-      <c r="X15" s="7">
+      <c r="Y15" s="7">
         <v>2.7836272409414802</v>
       </c>
-      <c r="Y15" s="7">
+      <c r="Z15" s="7">
         <v>84.064718444906106</v>
       </c>
-      <c r="Z15" s="7">
+      <c r="AA15" s="7">
         <v>75.974138934728501</v>
       </c>
-      <c r="AA15" s="7">
+      <c r="AB15" s="7">
         <v>1280.3042623915701</v>
       </c>
-      <c r="AB15" s="7">
+      <c r="AC15" s="7">
         <v>103.09805672184299</v>
       </c>
-      <c r="AC15" s="7">
+      <c r="AD15" s="7">
         <v>90.373460415450495</v>
       </c>
-      <c r="AD15" s="7">
+      <c r="AE15" s="7">
         <v>1280.3042623915701</v>
       </c>
-      <c r="AE15" s="7">
+      <c r="AF15" s="7">
         <v>135.105654751457</v>
       </c>
-      <c r="AF15" s="7">
+      <c r="AG15" s="7">
         <v>111.98622038818699</v>
       </c>
-      <c r="AG15" s="7">
+      <c r="AH15" s="7">
         <v>1280.3042623915701</v>
       </c>
-      <c r="AH15" s="7">
+      <c r="AI15" s="7">
         <v>1344.8879681139399</v>
       </c>
     </row>
-    <row r="16" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>5</v>
       </c>
@@ -2086,55 +2148,59 @@
         <v>0.4</v>
       </c>
       <c r="S16" s="7">
+        <f t="shared" si="0"/>
+        <v>9.7699200000000008</v>
+      </c>
+      <c r="T16" s="7">
         <v>0.15</v>
       </c>
-      <c r="T16" s="7" t="s">
+      <c r="U16" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U16" s="7">
+      <c r="V16" s="7">
         <v>72.595615589501804</v>
       </c>
-      <c r="V16" s="7">
+      <c r="W16" s="7">
         <v>66.108786396091105</v>
       </c>
-      <c r="W16" s="7">
+      <c r="X16" s="7">
         <v>1285.1822126531299</v>
       </c>
-      <c r="X16" s="7">
+      <c r="Y16" s="7">
         <v>2.7119036494740798</v>
       </c>
-      <c r="Y16" s="7">
+      <c r="Z16" s="7">
         <v>86.213565720463293</v>
       </c>
-      <c r="Z16" s="7">
+      <c r="AA16" s="7">
         <v>76.705526562280994</v>
       </c>
-      <c r="AA16" s="7">
+      <c r="AB16" s="7">
         <v>1285.1822126531299</v>
       </c>
-      <c r="AB16" s="7">
+      <c r="AC16" s="7">
         <v>106.84215319543399</v>
       </c>
-      <c r="AC16" s="7">
+      <c r="AD16" s="7">
         <v>91.549795614020695</v>
       </c>
-      <c r="AD16" s="7">
+      <c r="AE16" s="7">
         <v>1285.1822126531299</v>
       </c>
-      <c r="AE16" s="7">
+      <c r="AF16" s="7">
         <v>143.40033392381901</v>
       </c>
-      <c r="AF16" s="7">
+      <c r="AG16" s="7">
         <v>114.230085640732</v>
       </c>
-      <c r="AG16" s="7">
+      <c r="AH16" s="7">
         <v>1285.1822126531299</v>
       </c>
-      <c r="AH16" s="7">
+      <c r="AI16" s="7">
         <v>1348.59556605334</v>
       </c>
     </row>
-    <row r="17" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7">
         <v>5</v>
       </c>
@@ -2184,55 +2250,59 @@
         <v>0.4</v>
       </c>
       <c r="S17" s="7">
+        <f t="shared" si="0"/>
+        <v>9.759920000000001</v>
+      </c>
+      <c r="T17" s="7">
         <v>0.15</v>
       </c>
-      <c r="T17" s="7" t="s">
+      <c r="U17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U17" s="7">
+      <c r="V17" s="7">
         <v>74.275796994512902</v>
       </c>
-      <c r="V17" s="7">
+      <c r="W17" s="7">
         <v>66.653253769319207</v>
       </c>
-      <c r="W17" s="7">
+      <c r="X17" s="7">
         <v>1292.3295496426499</v>
       </c>
-      <c r="X17" s="7">
+      <c r="Y17" s="7">
         <v>2.6424095190928099</v>
       </c>
-      <c r="Y17" s="7">
+      <c r="Z17" s="7">
         <v>88.865898142309604</v>
       </c>
-      <c r="Z17" s="7">
+      <c r="AA17" s="7">
         <v>77.516218000949607</v>
       </c>
-      <c r="AA17" s="7">
+      <c r="AB17" s="7">
         <v>1292.3295496426499</v>
       </c>
-      <c r="AB17" s="7">
+      <c r="AC17" s="7">
         <v>111.67897856579</v>
       </c>
-      <c r="AC17" s="7">
+      <c r="AD17" s="7">
         <v>92.891741144138706</v>
       </c>
-      <c r="AD17" s="7">
+      <c r="AE17" s="7">
         <v>1292.3295496426499</v>
       </c>
-      <c r="AE17" s="7">
+      <c r="AF17" s="7">
         <v>155.40121695448701</v>
       </c>
-      <c r="AF17" s="7">
+      <c r="AG17" s="7">
         <v>116.974827728316</v>
       </c>
-      <c r="AG17" s="7">
+      <c r="AH17" s="7">
         <v>1292.3295496426499</v>
       </c>
-      <c r="AH17" s="7">
+      <c r="AI17" s="7">
         <v>1392.3922674960399</v>
       </c>
     </row>
-    <row r="18" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7">
         <v>5</v>
       </c>
@@ -2282,55 +2352,59 @@
         <v>0.39</v>
       </c>
       <c r="S18" s="7">
+        <f t="shared" si="0"/>
+        <v>9.750922000000001</v>
+      </c>
+      <c r="T18" s="7">
         <v>0.16</v>
       </c>
-      <c r="T18" s="7" t="s">
+      <c r="U18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U18" s="7">
+      <c r="V18" s="7">
         <v>76.715296736281104</v>
       </c>
-      <c r="V18" s="7">
+      <c r="W18" s="7">
         <v>67.282131454754307</v>
       </c>
-      <c r="W18" s="7">
+      <c r="X18" s="7">
         <v>1297.8234864769199</v>
       </c>
-      <c r="X18" s="7">
+      <c r="Y18" s="7">
         <v>2.5750807030804799</v>
       </c>
-      <c r="Y18" s="7">
+      <c r="Z18" s="7">
         <v>92.493966485304298</v>
       </c>
-      <c r="Z18" s="7">
+      <c r="AA18" s="7">
         <v>78.452327281221798</v>
       </c>
-      <c r="AA18" s="7">
+      <c r="AB18" s="7">
         <v>1297.8234864769199</v>
       </c>
-      <c r="AB18" s="7">
+      <c r="AC18" s="7">
         <v>118.050265855997</v>
       </c>
-      <c r="AC18" s="7">
+      <c r="AD18" s="7">
         <v>94.464148938629904</v>
       </c>
-      <c r="AD18" s="7">
+      <c r="AE18" s="7">
         <v>1297.8234864769199</v>
       </c>
-      <c r="AE18" s="7">
+      <c r="AF18" s="7">
         <v>172.16809084982799</v>
       </c>
-      <c r="AF18" s="7">
+      <c r="AG18" s="7">
         <v>120.42440667341</v>
       </c>
-      <c r="AG18" s="7">
+      <c r="AH18" s="7">
         <v>1297.8234864769199</v>
       </c>
-      <c r="AH18" s="7">
+      <c r="AI18" s="7">
         <v>1380.2325389909299</v>
       </c>
     </row>
-    <row r="19" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
         <v>5</v>
       </c>
@@ -2380,55 +2454,59 @@
         <v>0.39</v>
       </c>
       <c r="S19" s="7">
+        <f t="shared" si="0"/>
+        <v>9.7409220000000012</v>
+      </c>
+      <c r="T19" s="7">
         <v>0.17</v>
       </c>
-      <c r="T19" s="7" t="s">
+      <c r="U19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U19" s="7">
+      <c r="V19" s="7">
         <v>78.276856119876697</v>
       </c>
-      <c r="V19" s="7">
+      <c r="W19" s="7">
         <v>67.928879964467399</v>
       </c>
-      <c r="W19" s="7">
+      <c r="X19" s="7">
         <v>1305.0241825998</v>
       </c>
-      <c r="X19" s="7">
+      <c r="Y19" s="7">
         <v>2.5098545284732099</v>
       </c>
-      <c r="Y19" s="7">
+      <c r="Z19" s="7">
         <v>95.488372929423804</v>
       </c>
-      <c r="Z19" s="7">
+      <c r="AA19" s="7">
         <v>79.454447613468901</v>
       </c>
-      <c r="AA19" s="7">
+      <c r="AB19" s="7">
         <v>1305.0241825998</v>
       </c>
-      <c r="AB19" s="7">
+      <c r="AC19" s="7">
         <v>125.026999525976</v>
       </c>
-      <c r="AC19" s="7">
+      <c r="AD19" s="7">
         <v>96.261963679062006</v>
       </c>
-      <c r="AD19" s="7">
+      <c r="AE19" s="7">
         <v>1305.0241825998</v>
       </c>
-      <c r="AE19" s="7">
+      <c r="AF19" s="7">
         <v>143.95935904269299</v>
       </c>
-      <c r="AF19" s="7">
+      <c r="AG19" s="7">
         <v>121.80881563630901</v>
       </c>
-      <c r="AG19" s="7">
+      <c r="AH19" s="7">
         <v>1305.0241825998</v>
       </c>
-      <c r="AH19" s="7">
+      <c r="AI19" s="7">
         <v>1420.2353205659001</v>
       </c>
     </row>
-    <row r="20" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
         <v>5</v>
       </c>
@@ -2478,55 +2556,59 @@
         <v>0.38</v>
       </c>
       <c r="S20" s="7">
+        <f t="shared" si="0"/>
+        <v>9.7219240000000013</v>
+      </c>
+      <c r="T20" s="7">
         <v>0.18</v>
       </c>
-      <c r="T20" s="7" t="s">
+      <c r="U20" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U20" s="7">
+      <c r="V20" s="7">
         <v>80.6106442646646</v>
       </c>
-      <c r="V20" s="7">
+      <c r="W20" s="7">
         <v>68.633422425589501</v>
       </c>
-      <c r="W20" s="7">
+      <c r="X20" s="7">
         <v>1310.0268649177401</v>
       </c>
-      <c r="X20" s="7">
+      <c r="Y20" s="7">
         <v>2.4466697735401799</v>
       </c>
-      <c r="Y20" s="7">
+      <c r="Z20" s="7">
         <v>99.603824816529595</v>
       </c>
-      <c r="Z20" s="7">
+      <c r="AA20" s="7">
         <v>80.573857458083395</v>
       </c>
-      <c r="AA20" s="7">
+      <c r="AB20" s="7">
         <v>1310.0268649177401</v>
       </c>
-      <c r="AB20" s="7">
+      <c r="AC20" s="7">
         <v>134.544778009933</v>
       </c>
-      <c r="AC20" s="7">
+      <c r="AD20" s="7">
         <v>98.388786697443706</v>
       </c>
-      <c r="AD20" s="7">
+      <c r="AE20" s="7">
         <v>1310.0268649177401</v>
       </c>
-      <c r="AE20" s="7">
+      <c r="AF20" s="7">
         <v>115.179554238265</v>
       </c>
-      <c r="AF20" s="7">
+      <c r="AG20" s="7">
         <v>121.440523336418</v>
       </c>
-      <c r="AG20" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH20" s="7">
+      <c r="AH20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI20" s="7">
         <v>1395.0724643226499</v>
       </c>
     </row>
-    <row r="21" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>5</v>
       </c>
@@ -2576,55 +2658,59 @@
         <v>0.38</v>
       </c>
       <c r="S21" s="7">
+        <f t="shared" si="0"/>
+        <v>9.7119239999999998</v>
+      </c>
+      <c r="T21" s="7">
         <v>0.19</v>
       </c>
-      <c r="T21" s="7" t="s">
+      <c r="U21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U21" s="7">
+      <c r="V21" s="7">
         <v>83.523847295295397</v>
       </c>
-      <c r="V21" s="7">
+      <c r="W21" s="7">
         <v>69.417128997679299</v>
       </c>
-      <c r="W21" s="7">
+      <c r="X21" s="7">
         <v>1317.07367470189</v>
       </c>
-      <c r="X21" s="7">
+      <c r="Y21" s="7">
         <v>2.3854666454072699</v>
       </c>
-      <c r="Y21" s="7">
+      <c r="Z21" s="7">
         <v>105.02728110247</v>
       </c>
-      <c r="Z21" s="7">
+      <c r="AA21" s="7">
         <v>81.860879755156404</v>
       </c>
-      <c r="AA21" s="7">
+      <c r="AB21" s="7">
         <v>1317.07367470189</v>
       </c>
-      <c r="AB21" s="7">
+      <c r="AC21" s="7">
         <v>149.038964236379</v>
       </c>
-      <c r="AC21" s="7">
+      <c r="AD21" s="7">
         <v>101.054585515282</v>
       </c>
-      <c r="AD21" s="7">
+      <c r="AE21" s="7">
         <v>1317.07367470189</v>
       </c>
-      <c r="AE21" s="7">
+      <c r="AF21" s="7">
         <v>91.929174478784702</v>
       </c>
-      <c r="AF21" s="7">
+      <c r="AG21" s="7">
         <v>119.88729444917399</v>
       </c>
-      <c r="AG21" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH21" s="7">
+      <c r="AH21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI21" s="7">
         <v>1443.9162508166701</v>
       </c>
     </row>
-    <row r="22" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7">
         <v>5</v>
       </c>
@@ -2674,55 +2760,59 @@
         <v>0.38</v>
       </c>
       <c r="S22" s="7">
+        <f t="shared" si="0"/>
+        <v>9.701924</v>
+      </c>
+      <c r="T22" s="7">
         <v>0.21</v>
       </c>
-      <c r="T22" s="7" t="s">
+      <c r="U22" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U22" s="7">
+      <c r="V22" s="7">
         <v>87.016465105817502</v>
       </c>
-      <c r="V22" s="7">
+      <c r="W22" s="7">
         <v>70.297095803086194</v>
       </c>
-      <c r="W22" s="7">
+      <c r="X22" s="7">
         <v>1324.4233996978901</v>
       </c>
-      <c r="X22" s="7">
+      <c r="Y22" s="7">
         <v>2.3261867578254898</v>
       </c>
-      <c r="Y22" s="7">
+      <c r="Z22" s="7">
         <v>112.017386513123</v>
       </c>
-      <c r="Z22" s="7">
+      <c r="AA22" s="7">
         <v>83.3687050930547</v>
       </c>
-      <c r="AA22" s="7">
+      <c r="AB22" s="7">
         <v>1324.4233996978901</v>
       </c>
-      <c r="AB22" s="7">
+      <c r="AC22" s="7">
         <v>149.64734484014801</v>
       </c>
-      <c r="AC22" s="7">
+      <c r="AD22" s="7">
         <v>103.484223481526</v>
       </c>
-      <c r="AD22" s="7">
+      <c r="AE22" s="7">
         <v>1324.4233996978901</v>
       </c>
-      <c r="AE22" s="7">
+      <c r="AF22" s="7">
         <v>73.189765835032404</v>
       </c>
-      <c r="AF22" s="7">
+      <c r="AG22" s="7">
         <v>117.55241801846699</v>
       </c>
-      <c r="AG22" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH22" s="7">
+      <c r="AH22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI22" s="7">
         <v>1464.0681746218399</v>
       </c>
     </row>
-    <row r="23" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7">
         <v>5</v>
       </c>
@@ -2772,55 +2862,59 @@
         <v>0.37</v>
       </c>
       <c r="S23" s="7">
+        <f t="shared" si="0"/>
+        <v>9.6829260000000001</v>
+      </c>
+      <c r="T23" s="7">
         <v>0.22</v>
       </c>
-      <c r="T23" s="7" t="s">
+      <c r="U23" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U23" s="7">
+      <c r="V23" s="7">
         <v>90.883734492496998</v>
       </c>
-      <c r="V23" s="7">
+      <c r="W23" s="7">
         <v>71.277411931153395</v>
       </c>
-      <c r="W23" s="7">
+      <c r="X23" s="7">
         <v>1329.50990485338</v>
       </c>
-      <c r="X23" s="7">
+      <c r="Y23" s="7">
         <v>2.2687731090843402</v>
       </c>
-      <c r="Y23" s="7">
+      <c r="Z23" s="7">
         <v>120.536040144773</v>
       </c>
-      <c r="Z23" s="7">
+      <c r="AA23" s="7">
         <v>85.138578190755595</v>
       </c>
-      <c r="AA23" s="7">
+      <c r="AB23" s="7">
         <v>1329.50990485338</v>
       </c>
-      <c r="AB23" s="7">
+      <c r="AC23" s="7">
         <v>118.839496981387</v>
       </c>
-      <c r="AC23" s="7">
+      <c r="AD23" s="7">
         <v>104.215426981519</v>
       </c>
-      <c r="AD23" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE23" s="7">
+      <c r="AE23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF23" s="7">
         <v>58.122213697220403</v>
       </c>
-      <c r="AF23" s="7">
+      <c r="AG23" s="7">
         <v>114.722408288884</v>
       </c>
-      <c r="AG23" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH23" s="7">
+      <c r="AH23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI23" s="7">
         <v>1431.24000796327</v>
       </c>
     </row>
-    <row r="24" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7">
         <v>5</v>
       </c>
@@ -2870,55 +2964,59 @@
         <v>0.37</v>
       </c>
       <c r="S24" s="7">
+        <f t="shared" si="0"/>
+        <v>9.6729260000000004</v>
+      </c>
+      <c r="T24" s="7">
         <v>0.23</v>
       </c>
-      <c r="T24" s="7" t="s">
+      <c r="U24" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U24" s="7">
+      <c r="V24" s="7">
         <v>96.048484651952606</v>
       </c>
-      <c r="V24" s="7">
+      <c r="W24" s="7">
         <v>72.403369782098807</v>
       </c>
-      <c r="W24" s="7">
+      <c r="X24" s="7">
         <v>1336.90816875112</v>
       </c>
-      <c r="X24" s="7">
+      <c r="Y24" s="7">
         <v>2.2131700600708402</v>
       </c>
-      <c r="Y24" s="7">
+      <c r="Z24" s="7">
         <v>133.53229375594699</v>
       </c>
-      <c r="Z24" s="7">
+      <c r="AA24" s="7">
         <v>87.338292534627897</v>
       </c>
-      <c r="AA24" s="7">
+      <c r="AB24" s="7">
         <v>1336.90816875112</v>
       </c>
-      <c r="AB24" s="7">
+      <c r="AC24" s="7">
         <v>94.128755891534098</v>
       </c>
-      <c r="AC24" s="7">
+      <c r="AD24" s="7">
         <v>103.756941931974</v>
       </c>
-      <c r="AD24" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE24" s="7">
+      <c r="AE24" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF24" s="7">
         <v>46.036644414930002</v>
       </c>
-      <c r="AF24" s="7">
+      <c r="AG24" s="7">
         <v>111.600328112795</v>
       </c>
-      <c r="AG24" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH24" s="7">
+      <c r="AH24" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI24" s="7">
         <v>1492.27171060349</v>
       </c>
     </row>
-    <row r="25" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7">
         <v>5</v>
       </c>
@@ -2968,55 +3066,59 @@
         <v>0.37</v>
       </c>
       <c r="S25" s="7">
+        <f t="shared" si="0"/>
+        <v>9.6629260000000006</v>
+      </c>
+      <c r="T25" s="7">
         <v>0.25</v>
       </c>
-      <c r="T25" s="7" t="s">
+      <c r="U25" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U25" s="7">
+      <c r="V25" s="7">
         <v>102.76706543031</v>
       </c>
-      <c r="V25" s="7">
+      <c r="W25" s="7">
         <v>73.723530462455798</v>
       </c>
-      <c r="W25" s="7">
+      <c r="X25" s="7">
         <v>1344.8639507033699</v>
       </c>
-      <c r="X25" s="7">
+      <c r="Y25" s="7">
         <v>2.1593233124745201</v>
       </c>
-      <c r="Y25" s="7">
+      <c r="Z25" s="7">
         <v>153.88469019824899</v>
       </c>
-      <c r="Z25" s="7">
+      <c r="AA25" s="7">
         <v>90.231614172176606</v>
       </c>
-      <c r="AA25" s="7">
+      <c r="AB25" s="7">
         <v>1344.8639507033699</v>
       </c>
-      <c r="AB25" s="7">
+      <c r="AC25" s="7">
         <v>74.357986820524999</v>
       </c>
-      <c r="AC25" s="7">
+      <c r="AD25" s="7">
         <v>102.478726492346</v>
       </c>
-      <c r="AD25" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE25" s="7">
+      <c r="AE25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF25" s="7">
         <v>36.3671246501032</v>
       </c>
-      <c r="AF25" s="7">
+      <c r="AG25" s="7">
         <v>108.329319266591</v>
       </c>
-      <c r="AG25" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH25" s="7">
+      <c r="AH25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI25" s="7">
         <v>1519.8911536529099</v>
       </c>
     </row>
-    <row r="26" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7">
         <v>5</v>
       </c>
@@ -3066,55 +3168,59 @@
         <v>0.37</v>
       </c>
       <c r="S26" s="7">
+        <f t="shared" si="0"/>
+        <v>9.6529260000000008</v>
+      </c>
+      <c r="T26" s="7">
         <v>0.27</v>
       </c>
-      <c r="T26" s="7" t="s">
+      <c r="U26" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U26" s="7">
+      <c r="V26" s="7">
         <v>111.605161397008</v>
       </c>
-      <c r="V26" s="7">
+      <c r="W26" s="7">
         <v>75.3019317513955</v>
       </c>
-      <c r="W26" s="7">
+      <c r="X26" s="7">
         <v>1352.4874940759</v>
       </c>
-      <c r="X26" s="7">
+      <c r="Y26" s="7">
         <v>2.1071798871390701</v>
       </c>
-      <c r="Y26" s="7">
+      <c r="Z26" s="7">
         <v>121.232111361699</v>
       </c>
-      <c r="Z26" s="7">
+      <c r="AA26" s="7">
         <v>91.523301555073402</v>
       </c>
-      <c r="AA26" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB26" s="7">
+      <c r="AB26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC26" s="7">
         <v>58.580068798554102</v>
       </c>
-      <c r="AC26" s="7">
+      <c r="AD26" s="7">
         <v>100.649615755105</v>
       </c>
-      <c r="AD26" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE26" s="7">
+      <c r="AE26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF26" s="7">
         <v>28.6504349445431</v>
       </c>
-      <c r="AF26" s="7">
+      <c r="AG26" s="7">
         <v>105.00936575317201</v>
       </c>
-      <c r="AG26" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH26" s="7">
+      <c r="AH26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI26" s="7">
         <v>1527.82899164419</v>
       </c>
     </row>
-    <row r="27" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7">
         <v>5</v>
       </c>
@@ -3164,55 +3270,59 @@
         <v>0.37</v>
       </c>
       <c r="S27" s="7">
+        <f t="shared" si="0"/>
+        <v>9.6529260000000008</v>
+      </c>
+      <c r="T27" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="T27" s="7" t="s">
+      <c r="U27" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U27" s="7">
+      <c r="V27" s="7">
         <v>125.34460005014</v>
       </c>
-      <c r="V27" s="7">
+      <c r="W27" s="7">
         <v>77.303638483345296</v>
       </c>
-      <c r="W27" s="7">
+      <c r="X27" s="7">
         <v>1361.20610153558</v>
       </c>
-      <c r="X27" s="7">
+      <c r="Y27" s="7">
         <v>2.05668810256104</v>
       </c>
-      <c r="Y27" s="7">
+      <c r="Z27" s="7">
         <v>95.2421261394379</v>
       </c>
-      <c r="Z27" s="7">
+      <c r="AA27" s="7">
         <v>91.672054538447995</v>
       </c>
-      <c r="AA27" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB27" s="7">
+      <c r="AB27" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC27" s="7">
         <v>46.021555172976498</v>
       </c>
-      <c r="AC27" s="7">
+      <c r="AD27" s="7">
         <v>98.464493331819597</v>
       </c>
-      <c r="AD27" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE27" s="7">
+      <c r="AE27" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF27" s="7">
         <v>22.508296756431999</v>
       </c>
-      <c r="AF27" s="7">
+      <c r="AG27" s="7">
         <v>101.709322993303</v>
       </c>
-      <c r="AG27" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH27" s="7">
+      <c r="AH27" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI27" s="7">
         <v>1570.45268056792</v>
       </c>
     </row>
-    <row r="28" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7">
         <v>5</v>
       </c>
@@ -3262,55 +3372,59 @@
         <v>0.37</v>
       </c>
       <c r="S28" s="7">
+        <f t="shared" si="0"/>
+        <v>9.642926000000001</v>
+      </c>
+      <c r="T28" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="T28" s="7" t="s">
+      <c r="U28" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U28" s="7">
+      <c r="V28" s="7">
         <v>123.082389293246</v>
       </c>
-      <c r="V28" s="7">
+      <c r="W28" s="7">
         <v>77.612831476499096</v>
       </c>
-      <c r="W28" s="7">
+      <c r="X28" s="7">
         <v>1361.5883401635001</v>
       </c>
-      <c r="X28" s="7">
+      <c r="Y28" s="7">
         <v>2.04843113238269</v>
       </c>
-      <c r="Y28" s="7">
+      <c r="Z28" s="7">
         <v>90.965936133044494</v>
       </c>
-      <c r="Z28" s="7">
+      <c r="AA28" s="7">
         <v>91.667285363679596</v>
       </c>
-      <c r="AA28" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB28" s="7">
+      <c r="AB28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC28" s="7">
         <v>43.955275026928</v>
       </c>
-      <c r="AC28" s="7">
+      <c r="AD28" s="7">
         <v>98.0963341299192</v>
       </c>
-      <c r="AD28" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE28" s="7">
+      <c r="AE28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF28" s="7">
         <v>21.4977171153404</v>
       </c>
-      <c r="AF28" s="7">
+      <c r="AG28" s="7">
         <v>101.167568007238</v>
       </c>
-      <c r="AG28" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH28" s="7">
+      <c r="AH28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI28" s="7">
         <v>1417.7999030921601</v>
       </c>
     </row>
-    <row r="29" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7">
         <v>5</v>
       </c>
@@ -3357,55 +3471,59 @@
         <v>0.37</v>
       </c>
       <c r="S29" s="7">
+        <f t="shared" si="0"/>
+        <v>9.642926000000001</v>
+      </c>
+      <c r="T29" s="7">
         <v>0.3</v>
       </c>
-      <c r="T29" s="7" t="s">
+      <c r="U29" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U29" s="7">
+      <c r="V29" s="7">
         <v>146.79698884054201</v>
       </c>
-      <c r="V29" s="7">
+      <c r="W29" s="7">
         <v>79.821402653889706</v>
       </c>
-      <c r="W29" s="7">
+      <c r="X29" s="7">
         <v>1370.4808084814899</v>
       </c>
-      <c r="X29" s="7">
+      <c r="Y29" s="7">
         <v>2.00809343976037</v>
       </c>
-      <c r="Y29" s="7">
+      <c r="Z29" s="7">
         <v>73.953974028919006</v>
       </c>
-      <c r="Z29" s="7">
+      <c r="AA29" s="7">
         <v>91.101821963377702</v>
       </c>
-      <c r="AA29" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB29" s="7">
+      <c r="AB29" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC29" s="7">
         <v>35.734994943833499</v>
       </c>
-      <c r="AC29" s="7">
+      <c r="AD29" s="7">
         <v>96.105568302055701</v>
       </c>
-      <c r="AD29" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE29" s="7">
+      <c r="AE29" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF29" s="7">
         <v>17.477329215891</v>
       </c>
-      <c r="AF29" s="7">
+      <c r="AG29" s="7">
         <v>98.495918076590996</v>
       </c>
-      <c r="AG29" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH29" s="7">
+      <c r="AH29" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI29" s="7">
         <v>1640.1475886789001</v>
       </c>
     </row>
-    <row r="30" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7">
         <v>5</v>
       </c>
@@ -3452,55 +3570,59 @@
         <v>0.37</v>
       </c>
       <c r="S30" s="7">
+        <f t="shared" si="0"/>
+        <v>9.642926000000001</v>
+      </c>
+      <c r="T30" s="7">
         <v>0.31</v>
       </c>
-      <c r="T30" s="7" t="s">
+      <c r="U30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U30" s="7">
+      <c r="V30" s="7">
         <v>125.06430234996</v>
       </c>
-      <c r="V30" s="7">
+      <c r="W30" s="7">
         <v>81.497065605596006</v>
       </c>
-      <c r="W30" s="7">
+      <c r="X30" s="7">
         <v>1380.5201023529501</v>
       </c>
-      <c r="X30" s="7">
+      <c r="Y30" s="7">
         <v>1.9607201741253499</v>
       </c>
-      <c r="Y30" s="7">
+      <c r="Z30" s="7">
         <v>57.764875537962403</v>
       </c>
-      <c r="Z30" s="7">
+      <c r="AA30" s="7">
         <v>89.867120243917796</v>
       </c>
-      <c r="AA30" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB30" s="7">
+      <c r="AB30" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC30" s="7">
         <v>27.9123273953211</v>
       </c>
-      <c r="AC30" s="7">
+      <c r="AD30" s="7">
         <v>93.579892712917399</v>
       </c>
-      <c r="AD30" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE30" s="7">
+      <c r="AE30" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF30" s="7">
         <v>13.651406298965799</v>
       </c>
-      <c r="AF30" s="7">
+      <c r="AG30" s="7">
         <v>95.353528751493798</v>
       </c>
-      <c r="AG30" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH30" s="7">
+      <c r="AH30" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI30" s="7">
         <v>1641.5417430109701</v>
       </c>
     </row>
-    <row r="31" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="7">
         <v>5</v>
       </c>
@@ -3547,55 +3669,59 @@
         <v>0.37</v>
       </c>
       <c r="S31" s="7">
+        <f t="shared" si="0"/>
+        <v>9.642926000000001</v>
+      </c>
+      <c r="T31" s="7">
         <v>0.32</v>
       </c>
-      <c r="T31" s="7" t="s">
+      <c r="U31" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U31" s="7">
+      <c r="V31" s="7">
         <v>97.394695568452306</v>
       </c>
-      <c r="V31" s="7">
+      <c r="W31" s="7">
         <v>82.064838104269498</v>
       </c>
-      <c r="W31" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X31" s="7">
+      <c r="X31" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y31" s="7">
         <v>1.9148552199053399</v>
       </c>
-      <c r="Y31" s="7">
+      <c r="Z31" s="7">
         <v>44.984798714396497</v>
       </c>
-      <c r="Z31" s="7">
+      <c r="AA31" s="7">
         <v>88.264180189292105</v>
       </c>
-      <c r="AA31" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB31" s="7">
+      <c r="AB31" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC31" s="7">
         <v>21.736919154334</v>
       </c>
-      <c r="AC31" s="7">
+      <c r="AD31" s="7">
         <v>91.014072228682295</v>
       </c>
-      <c r="AD31" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE31" s="7">
+      <c r="AE31" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF31" s="7">
         <v>10.631127632636201</v>
       </c>
-      <c r="AF31" s="7">
+      <c r="AG31" s="7">
         <v>92.327728711534604</v>
       </c>
-      <c r="AG31" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH31" s="7">
+      <c r="AH31" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI31" s="7">
         <v>1665.6842981206701</v>
       </c>
     </row>
-    <row r="32" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7">
         <v>5</v>
       </c>
@@ -3642,55 +3768,59 @@
         <v>0.37</v>
       </c>
       <c r="S32" s="7">
+        <f t="shared" si="0"/>
+        <v>9.642926000000001</v>
+      </c>
+      <c r="T32" s="7">
         <v>0.33</v>
       </c>
-      <c r="T32" s="7" t="s">
+      <c r="U32" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U32" s="7">
+      <c r="V32" s="7">
         <v>75.614447192384901</v>
       </c>
-      <c r="V32" s="7">
+      <c r="W32" s="7">
         <v>81.842410831445903</v>
       </c>
-      <c r="W32" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X32" s="7">
+      <c r="X32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y32" s="7">
         <v>1.87045134958573</v>
       </c>
-      <c r="Y32" s="7">
+      <c r="Z32" s="7">
         <v>34.924907018771997</v>
       </c>
-      <c r="Z32" s="7">
+      <c r="AA32" s="7">
         <v>86.424894907549998</v>
       </c>
-      <c r="AA32" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB32" s="7">
+      <c r="AB32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC32" s="7">
         <v>16.8759203561074</v>
       </c>
-      <c r="AC32" s="7">
+      <c r="AD32" s="7">
         <v>88.457584233076304</v>
       </c>
-      <c r="AD32" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE32" s="7">
+      <c r="AE32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF32" s="7">
         <v>8.2537024658441194</v>
       </c>
-      <c r="AF32" s="7">
+      <c r="AG32" s="7">
         <v>89.428624358234899</v>
       </c>
-      <c r="AG32" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH32" s="7">
+      <c r="AH32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI32" s="7">
         <v>1683.3088592305101</v>
       </c>
     </row>
-    <row r="33" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7">
         <v>5</v>
       </c>
@@ -3737,55 +3867,59 @@
         <v>0.38</v>
       </c>
       <c r="S33" s="7">
+        <f t="shared" si="0"/>
+        <v>9.6419240000000013</v>
+      </c>
+      <c r="T33" s="7">
         <v>0.33</v>
       </c>
-      <c r="T33" s="7" t="s">
+      <c r="U33" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U33" s="7">
+      <c r="V33" s="7">
         <v>60.859472458199001</v>
       </c>
-      <c r="V33" s="7">
+      <c r="W33" s="7">
         <v>81.258574463702203</v>
       </c>
-      <c r="W33" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X33" s="7">
+      <c r="X33" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y33" s="7">
         <v>1.83477298540154</v>
       </c>
-      <c r="Y33" s="7">
+      <c r="Z33" s="7">
         <v>28.109858575123901</v>
       </c>
-      <c r="Z33" s="7">
+      <c r="AA33" s="7">
         <v>84.802317631119806</v>
       </c>
-      <c r="AA33" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB33" s="7">
+      <c r="AB33" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC33" s="7">
         <v>13.582848890055899</v>
       </c>
-      <c r="AC33" s="7">
+      <c r="AD33" s="7">
         <v>86.374244295606999</v>
       </c>
-      <c r="AD33" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE33" s="7">
+      <c r="AE33" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF33" s="7">
         <v>6.64312173862983</v>
       </c>
-      <c r="AF33" s="7">
+      <c r="AG33" s="7">
         <v>87.125172558896196</v>
       </c>
-      <c r="AG33" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH33" s="7">
+      <c r="AH33" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI33" s="7">
         <v>1735.35780483843</v>
       </c>
     </row>
-    <row r="34" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7">
         <v>5</v>
       </c>
@@ -3830,55 +3964,59 @@
         <v>0.38</v>
       </c>
       <c r="S34" s="7">
+        <f t="shared" si="0"/>
+        <v>9.6519240000000011</v>
+      </c>
+      <c r="T34" s="7">
         <v>0.34</v>
       </c>
-      <c r="T34" s="7" t="s">
+      <c r="U34" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U34" s="7">
+      <c r="V34" s="7">
         <v>57.9479122094465</v>
       </c>
-      <c r="V34" s="7">
+      <c r="W34" s="7">
         <v>81.126480710928007</v>
       </c>
-      <c r="W34" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X34" s="7">
+      <c r="X34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y34" s="7">
         <v>1.8276638180020199</v>
       </c>
-      <c r="Y34" s="7">
+      <c r="Z34" s="7">
         <v>26.765063040105101</v>
       </c>
-      <c r="Z34" s="7">
+      <c r="AA34" s="7">
         <v>84.473439855104004</v>
       </c>
-      <c r="AA34" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB34" s="7">
+      <c r="AB34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC34" s="7">
         <v>12.933035782979401</v>
       </c>
-      <c r="AC34" s="7">
+      <c r="AD34" s="7">
         <v>85.958077447368794</v>
       </c>
-      <c r="AD34" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE34" s="7">
+      <c r="AE34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF34" s="7">
         <v>6.3253100915587401</v>
       </c>
-      <c r="AF34" s="7">
+      <c r="AG34" s="7">
         <v>86.667306671581301</v>
       </c>
-      <c r="AG34" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH34" s="7">
+      <c r="AH34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI34" s="7">
         <v>1832.5104714685799</v>
       </c>
     </row>
-    <row r="35" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="7">
         <v>5</v>
       </c>
@@ -3923,55 +4061,59 @@
         <v>0.39</v>
       </c>
       <c r="S35" s="7">
+        <f t="shared" si="0"/>
+        <v>9.7609220000000008</v>
+      </c>
+      <c r="T35" s="7">
         <v>0.36</v>
       </c>
-      <c r="T35" s="7" t="s">
+      <c r="U35" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U35" s="7">
+      <c r="V35" s="7">
         <v>36.386949554293601</v>
       </c>
-      <c r="V35" s="7">
+      <c r="W35" s="7">
         <v>78.330260013638394</v>
       </c>
-      <c r="W35" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X35" s="7">
+      <c r="X35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y35" s="7">
         <v>1.74464511288974</v>
       </c>
-      <c r="Y35" s="7">
+      <c r="Z35" s="7">
         <v>16.806455341095699</v>
       </c>
-      <c r="Z35" s="7">
+      <c r="AA35" s="7">
         <v>80.244253322978494</v>
       </c>
-      <c r="AA35" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB35" s="7">
+      <c r="AB35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC35" s="7">
         <v>8.1209780072530808</v>
       </c>
-      <c r="AC35" s="7">
+      <c r="AD35" s="7">
         <v>81.093258732361605</v>
       </c>
-      <c r="AD35" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE35" s="7">
+      <c r="AE35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF35" s="7">
         <v>3.9718210793329001</v>
       </c>
-      <c r="AF35" s="7">
+      <c r="AG35" s="7">
         <v>81.498838822065807</v>
       </c>
-      <c r="AG35" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH35" s="7">
+      <c r="AH35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI35" s="7">
         <v>1884.48342483183</v>
       </c>
     </row>
-    <row r="36" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="7">
         <v>5</v>
       </c>
@@ -4016,55 +4158,59 @@
         <v>0.4</v>
       </c>
       <c r="S36" s="7">
+        <f t="shared" si="0"/>
+        <v>9.8399200000000011</v>
+      </c>
+      <c r="T36" s="7">
         <v>0.38</v>
       </c>
-      <c r="T36" s="7" t="s">
+      <c r="U36" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U36" s="7">
+      <c r="V36" s="7">
         <v>22.600948809736</v>
       </c>
-      <c r="V36" s="7">
+      <c r="W36" s="7">
         <v>75.052065236938205</v>
       </c>
-      <c r="W36" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X36" s="7">
+      <c r="X36" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y36" s="7">
         <v>1.66719697362088</v>
       </c>
-      <c r="Y36" s="7">
+      <c r="Z36" s="7">
         <v>10.438957964048299</v>
       </c>
-      <c r="Z36" s="7">
+      <c r="AA36" s="7">
         <v>76.138059478335606</v>
       </c>
-      <c r="AA36" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB36" s="7">
+      <c r="AB36" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC36" s="7">
         <v>5.0441658472374096</v>
       </c>
-      <c r="AC36" s="7">
+      <c r="AD36" s="7">
         <v>76.619782680295401</v>
       </c>
-      <c r="AD36" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE36" s="7">
+      <c r="AE36" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF36" s="7">
         <v>2.4670088038429898</v>
       </c>
-      <c r="AF36" s="7">
+      <c r="AG36" s="7">
         <v>76.849907644523299</v>
       </c>
-      <c r="AG36" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH36" s="7">
+      <c r="AH36" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI36" s="7">
         <v>1816.8688995898899</v>
       </c>
     </row>
-    <row r="37" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="7">
         <v>5</v>
       </c>
@@ -4109,55 +4255,59 @@
         <v>0.41</v>
       </c>
       <c r="S37" s="7">
+        <f t="shared" si="0"/>
+        <v>9.9089179999999999</v>
+      </c>
+      <c r="T37" s="7">
         <v>0.4</v>
       </c>
-      <c r="T37" s="7" t="s">
+      <c r="U37" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U37" s="7">
+      <c r="V37" s="7">
         <v>13.8787379826777</v>
       </c>
-      <c r="V37" s="7">
+      <c r="W37" s="7">
         <v>71.653547056145996</v>
       </c>
-      <c r="W37" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X37" s="7">
+      <c r="X37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y37" s="7">
         <v>1.5948692910761399</v>
       </c>
-      <c r="Y37" s="7">
+      <c r="Z37" s="7">
         <v>6.4103309827772401</v>
       </c>
-      <c r="Z37" s="7">
+      <c r="AA37" s="7">
         <v>72.264296784137898</v>
       </c>
-      <c r="AA37" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB37" s="7">
+      <c r="AB37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC37" s="7">
         <v>3.0975096100754098</v>
       </c>
-      <c r="AC37" s="7">
+      <c r="AD37" s="7">
         <v>72.535211954172098</v>
       </c>
-      <c r="AD37" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE37" s="7">
+      <c r="AE37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF37" s="7">
         <v>1.5149350178938801</v>
       </c>
-      <c r="AF37" s="7">
+      <c r="AG37" s="7">
         <v>72.664631387488299</v>
       </c>
-      <c r="AG37" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH37" s="7">
+      <c r="AH37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI37" s="7">
         <v>1814.6478333144901</v>
       </c>
     </row>
-    <row r="38" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7">
         <v>5</v>
       </c>
@@ -4202,55 +4352,59 @@
         <v>0.42</v>
       </c>
       <c r="S38" s="7">
+        <f t="shared" si="0"/>
+        <v>9.9579160000000009</v>
+      </c>
+      <c r="T38" s="7">
         <v>0.42</v>
       </c>
-      <c r="T38" s="7" t="s">
+      <c r="U38" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U38" s="7">
+      <c r="V38" s="7">
         <v>8.4210644313691603</v>
       </c>
-      <c r="V38" s="7">
+      <c r="W38" s="7">
         <v>68.325521654842007</v>
       </c>
-      <c r="W38" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X38" s="7">
+      <c r="X38" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y38" s="7">
         <v>1.52726260460138</v>
       </c>
-      <c r="Y38" s="7">
+      <c r="Z38" s="7">
         <v>3.88953306127291</v>
       </c>
-      <c r="Z38" s="7">
+      <c r="AA38" s="7">
         <v>68.665625009250306</v>
       </c>
-      <c r="AA38" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB38" s="7">
+      <c r="AB38" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC38" s="7">
         <v>1.8794452374406401</v>
       </c>
-      <c r="AC38" s="7">
+      <c r="AD38" s="7">
         <v>68.816487390133602</v>
       </c>
-      <c r="AD38" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE38" s="7">
+      <c r="AE38" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF38" s="7">
         <v>0.91920212132720103</v>
       </c>
-      <c r="AF38" s="7">
+      <c r="AG38" s="7">
         <v>68.888556162953506</v>
       </c>
-      <c r="AG38" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH38" s="7">
+      <c r="AH38" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI38" s="7">
         <v>1772.9691824461399</v>
       </c>
     </row>
-    <row r="39" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7">
         <v>5</v>
       </c>
@@ -4295,55 +4449,59 @@
         <v>0.43</v>
       </c>
       <c r="S39" s="7">
+        <f t="shared" si="0"/>
+        <v>9.9969140000000003</v>
+      </c>
+      <c r="T39" s="7">
         <v>0.43</v>
       </c>
-      <c r="T39" s="7" t="s">
+      <c r="U39" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U39" s="7">
+      <c r="V39" s="7">
         <v>5.04556213408926</v>
       </c>
-      <c r="V39" s="7">
+      <c r="W39" s="7">
         <v>65.161523678804301</v>
       </c>
-      <c r="W39" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X39" s="7">
+      <c r="X39" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y39" s="7">
         <v>1.4640184875845701</v>
       </c>
-      <c r="Y39" s="7">
+      <c r="Z39" s="7">
         <v>2.3304513215862102</v>
       </c>
-      <c r="Z39" s="7">
+      <c r="AA39" s="7">
         <v>65.348866324867103</v>
       </c>
-      <c r="AA39" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB39" s="7">
+      <c r="AB39" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC39" s="7">
         <v>1.1260877767186399</v>
       </c>
-      <c r="AC39" s="7">
+      <c r="AD39" s="7">
         <v>65.431967409462899</v>
       </c>
-      <c r="AD39" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE39" s="7">
+      <c r="AE39" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF39" s="7">
         <v>0.55074883403890296</v>
       </c>
-      <c r="AF39" s="7">
+      <c r="AG39" s="7">
         <v>65.471665796507807</v>
       </c>
-      <c r="AG39" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH39" s="7">
+      <c r="AH39" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI39" s="7">
         <v>1750.7754610486199</v>
       </c>
     </row>
-    <row r="40" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="7">
         <v>5</v>
       </c>
@@ -4388,55 +4546,59 @@
         <v>0.44</v>
       </c>
       <c r="S40" s="7">
+        <f t="shared" si="0"/>
+        <v>10.005911999999999</v>
+      </c>
+      <c r="T40" s="7">
         <v>0.45</v>
       </c>
-      <c r="T40" s="7" t="s">
+      <c r="U40" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U40" s="7">
+      <c r="V40" s="7">
         <v>2.9832372515180698</v>
       </c>
-      <c r="V40" s="7">
+      <c r="W40" s="7">
         <v>62.200652896552597</v>
       </c>
-      <c r="W40" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X40" s="7">
+      <c r="X40" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y40" s="7">
         <v>1.40481254437688</v>
       </c>
-      <c r="Y40" s="7">
+      <c r="Z40" s="7">
         <v>1.3779018096782201</v>
       </c>
-      <c r="Z40" s="7">
+      <c r="AA40" s="7">
         <v>62.3026299193819</v>
       </c>
-      <c r="AA40" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB40" s="7">
+      <c r="AB40" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC40" s="7">
         <v>0.66581025358685597</v>
       </c>
-      <c r="AC40" s="7">
+      <c r="AD40" s="7">
         <v>62.347864687754502</v>
       </c>
-      <c r="AD40" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE40" s="7">
+      <c r="AE40" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF40" s="7">
         <v>0.325635557400894</v>
       </c>
-      <c r="AF40" s="7">
+      <c r="AG40" s="7">
         <v>62.369473880359898</v>
       </c>
-      <c r="AG40" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH40" s="7">
+      <c r="AH40" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI40" s="7">
         <v>2044.3491453431</v>
       </c>
     </row>
-    <row r="41" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="7">
         <v>5</v>
       </c>
@@ -4481,55 +4643,59 @@
         <v>0.44</v>
       </c>
       <c r="S41" s="7">
+        <f t="shared" si="0"/>
+        <v>10.005911999999999</v>
+      </c>
+      <c r="T41" s="7">
         <v>0.46</v>
       </c>
-      <c r="T41" s="7" t="s">
+      <c r="U41" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U41" s="7">
+      <c r="V41" s="7">
         <v>1.7393524884288101</v>
       </c>
-      <c r="V41" s="7">
+      <c r="W41" s="7">
         <v>59.452411968910603</v>
       </c>
-      <c r="W41" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X41" s="7">
+      <c r="X41" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y41" s="7">
         <v>1.34934919016543</v>
       </c>
-      <c r="Y41" s="7">
+      <c r="Z41" s="7">
         <v>0.80337456910434801</v>
       </c>
-      <c r="Z41" s="7">
+      <c r="AA41" s="7">
         <v>59.507209221642</v>
       </c>
-      <c r="AA41" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB41" s="7">
+      <c r="AB41" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC41" s="7">
         <v>0.38819531393569301</v>
       </c>
-      <c r="AC41" s="7">
+      <c r="AD41" s="7">
         <v>59.531516079853603</v>
       </c>
-      <c r="AD41" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE41" s="7">
+      <c r="AE41" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF41" s="7">
         <v>0.18985919299510201</v>
       </c>
-      <c r="AF41" s="7">
+      <c r="AG41" s="7">
         <v>59.5431277582069</v>
       </c>
-      <c r="AG41" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH41" s="7">
+      <c r="AH41" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI41" s="7">
         <v>2118.1771703639001</v>
       </c>
     </row>
-    <row r="42" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="7">
         <v>5</v>
       </c>
@@ -4574,55 +4740,59 @@
         <v>0.44</v>
       </c>
       <c r="S42" s="7">
+        <f t="shared" si="0"/>
+        <v>9.9959120000000006</v>
+      </c>
+      <c r="T42" s="7">
         <v>0.47</v>
       </c>
-      <c r="T42" s="7" t="s">
+      <c r="U42" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U42" s="7">
+      <c r="V42" s="7">
         <v>0.99923550628737801</v>
       </c>
-      <c r="V42" s="7">
+      <c r="W42" s="7">
         <v>56.9109695140139</v>
       </c>
-      <c r="W42" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X42" s="7">
+      <c r="X42" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y42" s="7">
         <v>1.29735767356543</v>
       </c>
-      <c r="Y42" s="7">
+      <c r="Z42" s="7">
         <v>0.46152829839714499</v>
       </c>
-      <c r="Z42" s="7">
+      <c r="AA42" s="7">
         <v>56.940005703239997</v>
       </c>
-      <c r="AA42" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB42" s="7">
+      <c r="AB42" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC42" s="7">
         <v>0.223013186596419</v>
       </c>
-      <c r="AC42" s="7">
+      <c r="AD42" s="7">
         <v>56.952885519277203</v>
       </c>
-      <c r="AD42" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE42" s="7">
+      <c r="AE42" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF42" s="7">
         <v>0.109071650569889</v>
       </c>
-      <c r="AF42" s="7">
+      <c r="AG42" s="7">
         <v>56.959038362222699</v>
       </c>
-      <c r="AG42" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH42" s="7">
+      <c r="AH42" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI42" s="7">
         <v>1963.07054804466</v>
       </c>
     </row>
-    <row r="43" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="7">
         <v>5</v>
       </c>
@@ -4667,55 +4837,59 @@
         <v>0.45</v>
       </c>
       <c r="S43" s="7">
+        <f t="shared" si="0"/>
+        <v>9.9749099999999995</v>
+      </c>
+      <c r="T43" s="7">
         <v>0.48</v>
       </c>
-      <c r="T43" s="7" t="s">
+      <c r="U43" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U43" s="7">
+      <c r="V43" s="7">
         <v>0.56514139290023802</v>
       </c>
-      <c r="V43" s="7">
+      <c r="W43" s="7">
         <v>54.563226675634198</v>
       </c>
-      <c r="W43" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X43" s="7">
+      <c r="X43" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y43" s="7">
         <v>1.2485889818002001</v>
       </c>
-      <c r="Y43" s="7">
+      <c r="Z43" s="7">
         <v>0.26102829991313897</v>
       </c>
-      <c r="Z43" s="7">
+      <c r="AA43" s="7">
         <v>54.578381644768101</v>
       </c>
-      <c r="AA43" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB43" s="7">
+      <c r="AB43" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC43" s="7">
         <v>0.12613040881272899</v>
       </c>
-      <c r="AC43" s="7">
+      <c r="AD43" s="7">
         <v>54.585104056341201</v>
       </c>
-      <c r="AD43" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE43" s="7">
+      <c r="AE43" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF43" s="7">
         <v>6.1688064666576503E-2</v>
       </c>
-      <c r="AF43" s="7">
+      <c r="AG43" s="7">
         <v>54.588315433157902</v>
       </c>
-      <c r="AG43" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH43" s="7">
+      <c r="AH43" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI43" s="7">
         <v>1984.83560051532</v>
       </c>
     </row>
-    <row r="44" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7">
         <v>5</v>
       </c>
@@ -4760,55 +4934,59 @@
         <v>0.45</v>
       </c>
       <c r="S44" s="7">
+        <f t="shared" si="0"/>
+        <v>9.9549099999999999</v>
+      </c>
+      <c r="T44" s="7">
         <v>0.48</v>
       </c>
-      <c r="T44" s="7" t="s">
+      <c r="U44" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U44" s="7">
+      <c r="V44" s="7">
         <v>0.31437632832962098</v>
       </c>
-      <c r="V44" s="7">
+      <c r="W44" s="7">
         <v>52.393272661742003</v>
       </c>
-      <c r="W44" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X44" s="7">
+      <c r="X44" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y44" s="7">
         <v>1.2028133836033901</v>
       </c>
-      <c r="Y44" s="7">
+      <c r="Z44" s="7">
         <v>0.14520457985865801</v>
       </c>
-      <c r="Z44" s="7">
+      <c r="AA44" s="7">
         <v>52.401054562171701</v>
       </c>
-      <c r="AA44" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB44" s="7">
+      <c r="AB44" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC44" s="7">
         <v>7.0163706483732005E-2</v>
       </c>
-      <c r="AC44" s="7">
+      <c r="AD44" s="7">
         <v>52.4045064423469</v>
       </c>
-      <c r="AD44" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE44" s="7">
+      <c r="AE44" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF44" s="7">
         <v>3.4315779228476999E-2</v>
       </c>
-      <c r="AF44" s="7">
+      <c r="AG44" s="7">
         <v>52.4061554470007</v>
       </c>
-      <c r="AG44" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH44" s="7">
+      <c r="AH44" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI44" s="7">
         <v>2029.2258954860399</v>
       </c>
     </row>
-    <row r="45" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="7">
         <v>5</v>
       </c>
@@ -4856,55 +5034,59 @@
         <v>0.45</v>
       </c>
       <c r="S45" s="7">
+        <f t="shared" si="0"/>
+        <v>9.9349099999999986</v>
+      </c>
+      <c r="T45" s="7">
         <v>0.48</v>
       </c>
-      <c r="T45" s="7" t="s">
+      <c r="U45" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U45" s="7">
+      <c r="V45" s="7">
         <v>0.22484500322097101</v>
       </c>
-      <c r="V45" s="7">
+      <c r="W45" s="7">
         <v>51.410507933481</v>
       </c>
-      <c r="W45" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X45" s="7">
+      <c r="X45" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y45" s="7">
         <v>1.1819247407350499</v>
       </c>
-      <c r="Y45" s="7">
+      <c r="Z45" s="7">
         <v>0.103851725731042</v>
       </c>
-      <c r="Z45" s="7">
+      <c r="AA45" s="7">
         <v>51.4158639278902</v>
       </c>
-      <c r="AA45" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB45" s="7">
+      <c r="AB45" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC45" s="7">
         <v>5.0181764301887997E-2</v>
       </c>
-      <c r="AC45" s="7">
+      <c r="AD45" s="7">
         <v>51.418239729416698</v>
       </c>
-      <c r="AD45" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE45" s="7">
+      <c r="AE45" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF45" s="7">
         <v>2.4542978576514E-2</v>
       </c>
-      <c r="AF45" s="7">
+      <c r="AG45" s="7">
         <v>51.419374678364697</v>
       </c>
-      <c r="AG45" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH45" s="7">
+      <c r="AH45" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI45" s="7">
         <v>1903.9472347937301</v>
       </c>
     </row>
-    <row r="46" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="7">
         <v>5</v>
       </c>
@@ -4952,55 +5134,59 @@
         <v>0.45</v>
       </c>
       <c r="S46" s="7">
+        <f t="shared" si="0"/>
+        <v>9.914909999999999</v>
+      </c>
+      <c r="T46" s="7">
         <v>0.47</v>
       </c>
-      <c r="T46" s="7" t="s">
+      <c r="U46" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U46" s="7">
+      <c r="V46" s="7">
         <v>0.156162054207511</v>
       </c>
-      <c r="V46" s="7">
+      <c r="W46" s="7">
         <v>50.385421015895503</v>
       </c>
-      <c r="W46" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X46" s="7">
+      <c r="X46" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y46" s="7">
         <v>1.1599641029444001</v>
       </c>
-      <c r="Y46" s="7">
+      <c r="Z46" s="7">
         <v>7.2128348821771299E-2</v>
       </c>
-      <c r="Z46" s="7">
+      <c r="AA46" s="7">
         <v>50.3889892163089</v>
       </c>
-      <c r="AA46" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB46" s="7">
+      <c r="AB46" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC46" s="7">
         <v>3.4852842112922097E-2</v>
       </c>
-      <c r="AC46" s="7">
+      <c r="AD46" s="7">
         <v>50.390571991670598</v>
       </c>
-      <c r="AD46" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE46" s="7">
+      <c r="AE46" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF46" s="7">
         <v>1.7045884480308901E-2</v>
       </c>
-      <c r="AF46" s="7">
+      <c r="AG46" s="7">
         <v>50.391328102487101</v>
       </c>
-      <c r="AG46" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH46" s="7">
+      <c r="AH46" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI46" s="7">
         <v>1839.62961713254</v>
       </c>
     </row>
-    <row r="47" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="7">
         <v>5</v>
       </c>
@@ -5048,55 +5234,59 @@
         <v>0.46</v>
       </c>
       <c r="S47" s="7">
+        <f t="shared" si="0"/>
+        <v>9.8639079999999986</v>
+      </c>
+      <c r="T47" s="7">
         <v>0.45</v>
       </c>
-      <c r="T47" s="7" t="s">
+      <c r="U47" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U47" s="7">
+      <c r="V47" s="7">
         <v>8.3772064064670498E-2</v>
       </c>
-      <c r="V47" s="7">
+      <c r="W47" s="7">
         <v>48.522396980642498</v>
       </c>
-      <c r="W47" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X47" s="7">
+      <c r="X47" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y47" s="7">
         <v>1.1195161129837501</v>
       </c>
-      <c r="Y47" s="7">
+      <c r="Z47" s="7">
         <v>3.8692758551620701E-2</v>
       </c>
-      <c r="Z47" s="7">
+      <c r="AA47" s="7">
         <v>48.5241634215771</v>
       </c>
-      <c r="AA47" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB47" s="7">
+      <c r="AB47" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC47" s="7">
         <v>1.8696568363783299E-2</v>
       </c>
-      <c r="AC47" s="7">
+      <c r="AD47" s="7">
         <v>48.524946975992599</v>
       </c>
-      <c r="AD47" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE47" s="7">
+      <c r="AE47" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF47" s="7">
         <v>9.1441479427896398E-3</v>
       </c>
-      <c r="AF47" s="7">
+      <c r="AG47" s="7">
         <v>48.525321289355801</v>
       </c>
-      <c r="AG47" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH47" s="7">
+      <c r="AH47" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI47" s="7">
         <v>2376.6403921800802</v>
       </c>
     </row>
-    <row r="48" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="7">
         <v>5</v>
       </c>
@@ -5144,55 +5334,59 @@
         <v>0.46</v>
       </c>
       <c r="S48" s="7">
+        <f t="shared" si="0"/>
+        <v>9.8039079999999998</v>
+      </c>
+      <c r="T48" s="7">
         <v>0.42</v>
       </c>
-      <c r="T48" s="7" t="s">
+      <c r="U48" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U48" s="7">
+      <c r="V48" s="7">
         <v>4.4051115199016597E-2</v>
       </c>
-      <c r="V48" s="7">
+      <c r="W48" s="7">
         <v>46.791027485448097</v>
       </c>
-      <c r="W48" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X48" s="7">
+      <c r="X48" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y48" s="7">
         <v>1.08147812797124</v>
       </c>
-      <c r="Y48" s="7">
+      <c r="Z48" s="7">
         <v>2.0346390928237899E-2</v>
       </c>
-      <c r="Z48" s="7">
+      <c r="AA48" s="7">
         <v>46.791884241911099</v>
       </c>
-      <c r="AA48" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB48" s="7">
+      <c r="AB48" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC48" s="7">
         <v>9.8314956902995597E-3</v>
       </c>
-      <c r="AC48" s="7">
+      <c r="AD48" s="7">
         <v>46.792264280267503</v>
       </c>
-      <c r="AD48" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE48" s="7">
+      <c r="AE48" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF48" s="7">
         <v>4.8084038387035E-3</v>
       </c>
-      <c r="AF48" s="7">
+      <c r="AG48" s="7">
         <v>46.792445829158702</v>
       </c>
-      <c r="AG48" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH48" s="7">
+      <c r="AH48" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI48" s="7">
         <v>2459.1165734583401</v>
       </c>
     </row>
-    <row r="49" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="7">
         <v>5</v>
       </c>
@@ -5240,55 +5434,59 @@
         <v>0.46</v>
       </c>
       <c r="S49" s="7">
+        <f t="shared" si="0"/>
+        <v>9.7439079999999993</v>
+      </c>
+      <c r="T49" s="7">
         <v>0.4</v>
       </c>
-      <c r="T49" s="7" t="s">
+      <c r="U49" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U49" s="7">
+      <c r="V49" s="7">
         <v>2.2675345158395199E-2</v>
       </c>
-      <c r="V49" s="7">
+      <c r="W49" s="7">
         <v>45.178325687507098</v>
       </c>
-      <c r="W49" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X49" s="7">
+      <c r="X49" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y49" s="7">
         <v>1.0456788685330101</v>
       </c>
-      <c r="Y49" s="7">
+      <c r="Z49" s="7">
         <v>1.0473320254006499E-2</v>
       </c>
-      <c r="Z49" s="7">
+      <c r="AA49" s="7">
         <v>45.178732141164303</v>
       </c>
-      <c r="AA49" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB49" s="7">
+      <c r="AB49" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC49" s="7">
         <v>5.0607699077228801E-3</v>
       </c>
-      <c r="AC49" s="7">
+      <c r="AD49" s="7">
         <v>45.178912435082701</v>
       </c>
-      <c r="AD49" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE49" s="7">
+      <c r="AE49" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF49" s="7">
         <v>2.4751295446429002E-3</v>
       </c>
-      <c r="AF49" s="7">
+      <c r="AG49" s="7">
         <v>45.178998563654801</v>
       </c>
-      <c r="AG49" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH49" s="7">
+      <c r="AH49" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI49" s="7">
         <v>2281.18388656567</v>
       </c>
     </row>
-    <row r="50" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="7">
         <v>5</v>
       </c>
@@ -5336,55 +5534,59 @@
         <v>0.46</v>
       </c>
       <c r="S50" s="7">
+        <f t="shared" si="0"/>
+        <v>9.6739079999999991</v>
+      </c>
+      <c r="T50" s="7">
         <v>0.38</v>
       </c>
-      <c r="T50" s="7" t="s">
+      <c r="U50" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U50" s="7">
+      <c r="V50" s="7">
         <v>1.14085330328176E-2</v>
       </c>
-      <c r="V50" s="7">
+      <c r="W50" s="7">
         <v>43.672761782358002</v>
       </c>
-      <c r="W50" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X50" s="7">
+      <c r="X50" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y50" s="7">
         <v>1.0119595208604699</v>
       </c>
-      <c r="Y50" s="7">
+      <c r="Z50" s="7">
         <v>5.26938925279703E-3</v>
       </c>
-      <c r="Z50" s="7">
+      <c r="AA50" s="7">
         <v>43.672950049433901</v>
       </c>
-      <c r="AA50" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB50" s="7">
+      <c r="AB50" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC50" s="7">
         <v>2.5461998598230698E-3</v>
       </c>
-      <c r="AC50" s="7">
+      <c r="AD50" s="7">
         <v>43.673033560575298</v>
       </c>
-      <c r="AD50" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE50" s="7">
+      <c r="AE50" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF50" s="7">
         <v>1.24529955214846E-3</v>
       </c>
-      <c r="AF50" s="7">
+      <c r="AG50" s="7">
         <v>43.673073454851398</v>
       </c>
-      <c r="AG50" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH50" s="7">
+      <c r="AH50" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI50" s="7">
         <v>2413.58427593433</v>
       </c>
     </row>
-    <row r="51" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="7">
         <v>5</v>
       </c>
@@ -5432,55 +5634,59 @@
         <v>0.47</v>
       </c>
       <c r="S51" s="7">
+        <f t="shared" si="0"/>
+        <v>9.6029059999999991</v>
+      </c>
+      <c r="T51" s="7">
         <v>0.37</v>
       </c>
-      <c r="T51" s="7" t="s">
+      <c r="U51" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U51" s="7">
+      <c r="V51" s="7">
         <v>5.6007739542113999E-3</v>
       </c>
-      <c r="V51" s="7">
+      <c r="W51" s="7">
         <v>42.264143685312703</v>
       </c>
-      <c r="W51" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X51" s="7">
+      <c r="X51" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y51" s="7">
         <v>0.980172768952285</v>
       </c>
-      <c r="Y51" s="7">
+      <c r="Z51" s="7">
         <v>2.5868933364852002E-3</v>
       </c>
-      <c r="Z51" s="7">
+      <c r="AA51" s="7">
         <v>42.2642286573017</v>
       </c>
-      <c r="AA51" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB51" s="7">
+      <c r="AB51" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC51" s="7">
         <v>1.2500020656548701E-3</v>
       </c>
-      <c r="AC51" s="7">
+      <c r="AD51" s="7">
         <v>42.264266349010398</v>
       </c>
-      <c r="AD51" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE51" s="7">
+      <c r="AE51" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF51" s="7">
         <v>6.11353035206288E-4</v>
       </c>
-      <c r="AF51" s="7">
+      <c r="AG51" s="7">
         <v>42.2642843547928</v>
       </c>
-      <c r="AG51" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH51" s="7">
+      <c r="AH51" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI51" s="7">
         <v>2552.93270836898</v>
       </c>
     </row>
-    <row r="52" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="7">
         <v>5</v>
       </c>
@@ -5528,51 +5734,55 @@
         <v>0.47</v>
       </c>
       <c r="S52" s="7">
+        <f t="shared" si="0"/>
+        <v>9.5529060000000001</v>
+      </c>
+      <c r="T52" s="7">
         <v>0.36</v>
       </c>
-      <c r="T52" s="7" t="s">
+      <c r="U52" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U52" s="7">
+      <c r="V52" s="7">
         <v>3.2973247534493402E-3</v>
       </c>
-      <c r="V52" s="7">
+      <c r="W52" s="7">
         <v>41.409309877766603</v>
       </c>
-      <c r="W52" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X52" s="7">
+      <c r="X52" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y52" s="7">
         <v>0.96079757185375303</v>
       </c>
-      <c r="Y52" s="7">
+      <c r="Z52" s="7">
         <v>1.5229729859945499E-3</v>
       </c>
-      <c r="Z52" s="7">
+      <c r="AA52" s="7">
         <v>41.409357240172703</v>
       </c>
-      <c r="AA52" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB52" s="7">
+      <c r="AB52" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC52" s="7">
         <v>7.3590949869480201E-4</v>
       </c>
-      <c r="AC52" s="7">
+      <c r="AD52" s="7">
         <v>41.4093782490962</v>
       </c>
-      <c r="AD52" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE52" s="7">
+      <c r="AE52" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF52" s="7">
         <v>3.5991980975527802E-4</v>
       </c>
-      <c r="AF52" s="7">
+      <c r="AG52" s="7">
         <v>41.409388285311501</v>
       </c>
-      <c r="AG52" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH52" s="7">
+      <c r="AH52" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI52" s="7">
         <v>2178.6298838958901</v>
       </c>
     </row>

</xml_diff>